<commit_message>
Doctor and pharmacy done
</commit_message>
<xml_diff>
--- a/backend/data/data-s.xlsx
+++ b/backend/data/data-s.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meditrack\Meditrack\backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FULL STACK\FSPRO\Meditrack\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988B91ED-84B3-40A3-B3C2-BBE76026782E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11496" yWindow="0" windowWidth="11640" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11496" yWindow="0" windowWidth="11640" windowHeight="12336"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Dhanu</t>
   </si>
@@ -66,18 +65,9 @@
     <t>department</t>
   </si>
   <si>
-    <t>phone</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>rollNo</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -87,25 +77,34 @@
     <t>Male</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Coimbatore</t>
-  </si>
-  <si>
-    <t>Coimabatore</t>
-  </si>
-  <si>
-    <t>Erode</t>
+    <t>year</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>1nd</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>regno</t>
+  </si>
+  <si>
+    <t>mobile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,11 +415,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,211 +431,184 @@
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2024175052</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>9865234175</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2024175052</v>
+        <v>2024175053</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>9865234175</v>
+        <v>6589742351</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>20</v>
+      <c r="E3" t="s">
+        <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2024175054</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>9658413457</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2024175053</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>6589742351</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>21</v>
-      </c>
       <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2024175054</v>
+        <v>2024175055</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>9658413457</v>
+        <v>7569841235</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5">
-        <v>22</v>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2024175056</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>8654123975</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2024175055</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>7569841235</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>20</v>
-      </c>
       <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2024175056</v>
+        <v>2024175057</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>8654123975</v>
+        <v>9574621574</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2024175057</v>
+        <v>2024175058</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>9574621574</v>
+        <v>7896542856</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2024175058</v>
+        <v>2024175059</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>7896542856</v>
+        <v>9865742563</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9">
-        <v>21</v>
+      <c r="E9" t="s">
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2024175059</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>9865742563</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>